<commit_message>
Added CSV support and Pandas analysis for Day 25
</commit_message>
<xml_diff>
--- a/reddit_posts.xlsx
+++ b/reddit_posts.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,102 +436,527 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
+          <t>Date Posted</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Title</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>URL</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Score</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
           <t>Date Scraped</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Title</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>URL</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2025-02-25</t>
+          <t>2025-03-07</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>I Built an Open-Source Algo Trading Framework for Instant Backtests &amp; Live Deployment</t>
+          <t>PREMIUM LITE? REALLY YOUTUBE?</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>https://www.reddit.com/r/Python/comments/1iwccvr/i_built_an_opensource_algo_trading_framework_for/</t>
+          <t>https://i.redd.it/ps8fhv549cne1.jpeg</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
+        <v>7619</v>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>2025-03-09</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2025-02-25</t>
+          <t>2025-03-04</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Is UV package manager taking over?</t>
+          <t>I Thought it was Supposed to be Bigger?</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>https://www.reddit.com/r/Python/comments/1isv37n/is_uv_package_manager_taking_over/</t>
+          <t>https://i.redd.it/2zukjeomekme1.jpeg</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
+        <v>7410</v>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>2025-03-09</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2025-02-25</t>
+          <t>2025-03-06</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>New to coding. Is it always this difficult?</t>
+          <t>How can someone donate $500 in low effort Shorts just like that?</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>https://www.reddit.com/r/Python/comments/1iuyt0y/new_to_coding_is_it_always_this_difficult/</t>
+          <t>https://i.redd.it/g1gwn7bbozme1.jpeg</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>5854</v>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>2025-03-09</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2025-02-25</t>
+          <t>2025-03-03</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>What the hell is going on with type hinting these days</t>
+          <t>Ublock Origin is gone.</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>https://www.reddit.com/r/Python/comments/1itzac1/what_the_hell_is_going_on_with_type_hinting_these/</t>
+          <t>https://www.reddit.com/r/youtube/comments/1j2ec76/ublock_origin_is_gone/</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>4609</v>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>2025-03-09</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2025-02-25</t>
+          <t>2025-03-03</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Happy Birthday, Python! 🎉🐍</t>
+          <t>Stay in School</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>https://www.reddit.com/r/Python/comments/1itu5mn/happy_birthday_python/</t>
+          <t>https://www.reddit.com/gallery/1j2ve1c</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>2635</v>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>2025-03-09</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>2025-03-02</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>The fact that he doesn't even address the costume in the video is hilarious</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ytrmm5srbbme1.jpeg</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>2286</v>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>2025-03-09</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>2025-03-04</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>I painted "Dorito Wars" by VanossGaming</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j1b3r48i7pme1.jpeg</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>2114</v>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>2025-03-09</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>2025-03-02</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Who is the YouTuber you would rate the lowest?</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cuucddozc9me1.png</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>1918</v>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>2025-03-09</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>2025-03-06</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>I think my channel got shadow banned</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5j2k17r0b5ne1.jpeg</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>1833</v>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>2025-03-09</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>2025-03-06</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Bro waited 10 years for a song title</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ourctbrop5ne1.jpeg</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
+        <v>1785</v>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>2025-03-09</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>2025-03-05</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Stop posting porn noone fucking wants to see it</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/youtube/comments/1j4egrw/stop_posting_porn_noone_fucking_wants_to_see_it/</t>
+        </is>
+      </c>
+      <c r="D12" t="n">
+        <v>1291</v>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>2025-03-09</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>2025-03-08</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Popular YouTuber who doesn't deserve their fame?</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j6mlcx</t>
+        </is>
+      </c>
+      <c r="D13" t="n">
+        <v>1289</v>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>2025-03-09</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>2025-03-08</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Grandpa won’t stop watching AI-generated cheating stories at full volume on his TV and he’s driving my Grandma insane.</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/youtube/comments/1j6o6u9/grandpa_wont_stop_watching_aigenerated_cheating/</t>
+        </is>
+      </c>
+      <c r="D14" t="n">
+        <v>1290</v>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>2025-03-09</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>2025-03-05</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Where's the 'Nudity &amp; Sexual content' report button?</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dqfx2ln0rume1.jpeg</t>
+        </is>
+      </c>
+      <c r="D15" t="n">
+        <v>1144</v>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>2025-03-09</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>2025-03-07</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Who the FUCK asked for this</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pzqi0nwxlane1.png</t>
+        </is>
+      </c>
+      <c r="D16" t="n">
+        <v>1138</v>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>2025-03-09</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>2025-03-02</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>This is the worst thumbnail i've ever seen</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sjdc5y21u8me1.png</t>
+        </is>
+      </c>
+      <c r="D17" t="n">
+        <v>1076</v>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>2025-03-09</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>2025-03-06</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Me when non-predatory Minecraft YouTuber</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vpeklffxfzme1.jpeg</t>
+        </is>
+      </c>
+      <c r="D18" t="n">
+        <v>941</v>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>2025-03-09</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>2025-03-03</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>I just got a 43 minute unskippable add what the hell youtube</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0axg0m2oqeme1.jpeg</t>
+        </is>
+      </c>
+      <c r="D19" t="n">
+        <v>835</v>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>2025-03-09</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>2025-03-02</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>People are flooding Markiplier's video about him losing his niece in a car crash with disgusting comments. These aren't even a quarter of the ones made on that video.</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j1tdiy</t>
+        </is>
+      </c>
+      <c r="D20" t="n">
+        <v>827</v>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>2025-03-09</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>2025-03-07</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>People who use AI voice to narrate their videos are so annoying.</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/youtube/comments/1j5us1j/people_who_use_ai_voice_to_narrate_their_videos/</t>
+        </is>
+      </c>
+      <c r="D21" t="n">
+        <v>613</v>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>2025-03-09</t>
         </is>
       </c>
     </row>

</xml_diff>